<commit_message>
Wijzigingen documentatie einde van de week
</commit_message>
<xml_diff>
--- a/Planning_Urenverdeling/Algemene planning.xlsx
+++ b/Planning_Urenverdeling/Algemene planning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>GroepsProject Robotica</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Urenverdeling op orde maken</t>
   </si>
   <si>
-    <t>Bug fix (probleem met kruispunt lichtwaardes en B = control)</t>
-  </si>
-  <si>
     <t>vergadering met team (documentatie check)</t>
   </si>
   <si>
@@ -163,6 +160,15 @@
   </si>
   <si>
     <t>Documentatie van het einde van de week oporde maken</t>
+  </si>
+  <si>
+    <t>Bug fix (probleem met kruispunt lichtwaardes en B = control) + belbin test in teamcontract</t>
+  </si>
+  <si>
+    <t>Documentatie tot nu toe op hu intranet zetten</t>
+  </si>
+  <si>
+    <t>activity diagrams</t>
   </si>
 </sst>
 </file>
@@ -688,7 +694,7 @@
   <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1032,7 +1038,7 @@
         <v>26</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1043,7 +1049,7 @@
         <v>26</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1076,7 +1082,7 @@
         <v>27</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1098,7 +1104,7 @@
         <v>27</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1108,7 +1114,9 @@
       <c r="B41" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="26"/>
+      <c r="C41" s="26" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="5">
@@ -1129,7 +1137,7 @@
         <v>42461</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1140,7 +1148,7 @@
         <v>42461</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1151,7 +1159,7 @@
         <v>42461</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1162,14 +1170,14 @@
         <v>42461</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="9" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1191,7 +1199,7 @@
         <v>42464</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1202,7 +1210,7 @@
         <v>42464</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:3">

</xml_diff>

<commit_message>
changes in the planning
</commit_message>
<xml_diff>
--- a/Planning_Urenverdeling/Algemene planning.xlsx
+++ b/Planning_Urenverdeling/Algemene planning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
   <si>
     <t>GroepsProject Robotica</t>
   </si>
@@ -169,6 +169,39 @@
   </si>
   <si>
     <t>activity diagrams</t>
+  </si>
+  <si>
+    <t>activity diagrams maken</t>
+  </si>
+  <si>
+    <t>Use case diagram afmaken</t>
+  </si>
+  <si>
+    <t>Activity diagrams afmaken</t>
+  </si>
+  <si>
+    <t>Beginnen aan het paper</t>
+  </si>
+  <si>
+    <t>Code commenten</t>
+  </si>
+  <si>
+    <t>Paper amaken</t>
+  </si>
+  <si>
+    <t>Code een laatste keer checken</t>
+  </si>
+  <si>
+    <t>Testen van de robot</t>
+  </si>
+  <si>
+    <t>Code afmaken</t>
+  </si>
+  <si>
+    <t>Code testen</t>
+  </si>
+  <si>
+    <t>Werken aan de could haves</t>
   </si>
 </sst>
 </file>
@@ -290,8 +323,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -359,9 +394,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -693,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1187,7 +1224,7 @@
       <c r="B48" s="10">
         <v>42464</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1198,7 +1235,7 @@
       <c r="B49" s="10">
         <v>42464</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="13" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1209,7 +1246,7 @@
       <c r="B50" s="10">
         <v>42464</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="13" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1220,7 +1257,9 @@
       <c r="B51" s="10">
         <v>42464</v>
       </c>
-      <c r="C51" s="7"/>
+      <c r="C51" s="13" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="5">
@@ -1229,7 +1268,7 @@
       <c r="B52" s="10">
         <v>42464</v>
       </c>
-      <c r="C52" s="7"/>
+      <c r="C52" s="13"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="5">
@@ -1238,7 +1277,7 @@
       <c r="B53" s="10">
         <v>42464</v>
       </c>
-      <c r="C53" s="7"/>
+      <c r="C53" s="13"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="5">
@@ -1247,7 +1286,9 @@
       <c r="B54" s="10">
         <v>42465</v>
       </c>
-      <c r="C54" s="7"/>
+      <c r="C54" s="28" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="5">
@@ -1256,7 +1297,7 @@
       <c r="B55" s="6">
         <v>42465</v>
       </c>
-      <c r="C55" s="7"/>
+      <c r="C55" s="28"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="5">
@@ -1265,7 +1306,7 @@
       <c r="B56" s="10">
         <v>42465</v>
       </c>
-      <c r="C56" s="7"/>
+      <c r="C56" s="28"/>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="5">
@@ -1274,7 +1315,9 @@
       <c r="B57" s="6">
         <v>42465</v>
       </c>
-      <c r="C57" s="7"/>
+      <c r="C57" s="28" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="5">
@@ -1283,7 +1326,9 @@
       <c r="B58" s="10">
         <v>42465</v>
       </c>
-      <c r="C58" s="7"/>
+      <c r="C58" s="28" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="5">
@@ -1292,7 +1337,9 @@
       <c r="B59" s="6">
         <v>42465</v>
       </c>
-      <c r="C59" s="7"/>
+      <c r="C59" s="28" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="5">
@@ -1301,7 +1348,9 @@
       <c r="B60" s="10">
         <v>42466</v>
       </c>
-      <c r="C60" s="7"/>
+      <c r="C60" s="21" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="5">
@@ -1310,7 +1359,9 @@
       <c r="B61" s="10">
         <v>42466</v>
       </c>
-      <c r="C61" s="7"/>
+      <c r="C61" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="5">
@@ -1319,7 +1370,9 @@
       <c r="B62" s="10">
         <v>42466</v>
       </c>
-      <c r="C62" s="7"/>
+      <c r="C62" s="21" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="5">
@@ -1328,7 +1381,9 @@
       <c r="B63" s="10">
         <v>42466</v>
       </c>
-      <c r="C63" s="7"/>
+      <c r="C63" s="21" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="5">
@@ -1337,7 +1392,7 @@
       <c r="B64" s="10">
         <v>42466</v>
       </c>
-      <c r="C64" s="7"/>
+      <c r="C64" s="21"/>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="5">
@@ -1346,7 +1401,9 @@
       <c r="B65" s="10">
         <v>42467</v>
       </c>
-      <c r="C65" s="7"/>
+      <c r="C65" s="26" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="5">
@@ -1355,7 +1412,9 @@
       <c r="B66" s="6">
         <v>42467</v>
       </c>
-      <c r="C66" s="7"/>
+      <c r="C66" s="26" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="5">
@@ -1364,7 +1423,9 @@
       <c r="B67" s="10">
         <v>42467</v>
       </c>
-      <c r="C67" s="7"/>
+      <c r="C67" s="26" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="5">
@@ -1373,7 +1434,7 @@
       <c r="B68" s="6">
         <v>42467</v>
       </c>
-      <c r="C68" s="7"/>
+      <c r="C68" s="26"/>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="5">

</xml_diff>